<commit_message>
Corrigindo o problema da primeira linha sumir
</commit_message>
<xml_diff>
--- a/tabela_de_palavras.xlsx
+++ b/tabela_de_palavras.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -424,510 +424,542 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>extensão</t>
+          <t>exceção</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>compreensão</t>
+          <t>concessão</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>ascensão</t>
+          <t>impressão</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>determinação</t>
+          <t>presunção</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>acepção</t>
+          <t>concepção</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>resignação</t>
+          <t>inspiração</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>gratidão</t>
+          <t>extensão</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>compreensão</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>inserção</t>
+          <t>ascensão</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>remissão</t>
+          <t>determinação</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>alusão</t>
+          <t>acepção</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>descrição</t>
+          <t>resignação</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>compaixão</t>
+          <t>gratidão</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>disposição</t>
+          <t>não</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>pretensão</t>
+          <t>inserção</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>discrição</t>
+          <t>remissão</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>tribulação</t>
+          <t>alusão</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>paixão</t>
+          <t>descrição</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>percepção</t>
+          <t>compaixão</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>transgressão</t>
+          <t>disposição</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>resolução</t>
+          <t>pretensão</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>seção</t>
+          <t>discrição</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>dissensão</t>
+          <t>tribulação</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>comunhão</t>
+          <t>paixão</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>expressão</t>
+          <t>percepção</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>intervenção</t>
+          <t>transgressão</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>supressão</t>
+          <t>resolução</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>adesão</t>
+          <t>seção</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>consideração</t>
+          <t>dissensão</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>restrição</t>
+          <t>comunhão</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>redenção</t>
+          <t>expressão</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>proposição</t>
+          <t>intervenção</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>sessão</t>
+          <t>supressão</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>ação</t>
+          <t>adesão</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>reflexão</t>
+          <t>consideração</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>emulação</t>
+          <t>restrição</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>ambição</t>
+          <t>redenção</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>dissolução</t>
+          <t>proposição</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>relação</t>
+          <t>sessão</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>imersão</t>
+          <t>ação</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>designação</t>
+          <t>reflexão</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>submissão</t>
+          <t>emulação</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>dimensão</t>
+          <t>ambição</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>razão</t>
+          <t>dissolução</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>disseminação</t>
+          <t>relação</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>bom</t>
+          <t>imersão</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>dom</t>
+          <t>designação</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>com</t>
+          <t>submissão</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>som</t>
+          <t>dimensão</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>tom</t>
+          <t>razão</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>marrom</t>
+          <t>disseminação</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>bombom</t>
+          <t>bom</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>armagedom</t>
+          <t>dom</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>batom</t>
+          <t>com</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>garçom</t>
+          <t>som</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>maçom</t>
+          <t>tom</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>boom</t>
+          <t>marrom</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>guidom</t>
+          <t>bombom</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>ultrassom</t>
+          <t>armagedom</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>cupom</t>
+          <t>batom</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>zoom</t>
+          <t>garçom</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>showroom</t>
+          <t>maçom</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>moletom</t>
+          <t>boom</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>edredom</t>
+          <t>guidom</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>shalom</t>
+          <t>ultrassom</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>nom</t>
+          <t>cupom</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>crepom</t>
+          <t>zoom</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>trom</t>
+          <t>showroom</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>pompom</t>
+          <t>moletom</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>iândom</t>
+          <t>edredom</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>pogrom</t>
+          <t>shalom</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>bem-bom</t>
+          <t>nom</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>homem-bom</t>
+          <t>crepom</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>jetom</t>
+          <t>trom</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>burbom</t>
+          <t>pompom</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>condom</t>
+          <t>iândom</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>califom</t>
+          <t>pogrom</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>ronrom</t>
+          <t>bem-bom</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>champinhom</t>
+          <t>homem-bom</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>pistom</t>
+          <t>jetom</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>acordeom</t>
+          <t>burbom</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>infrassom</t>
+          <t>condom</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>ano-bom</t>
+          <t>califom</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>calom</t>
+          <t>ronrom</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>creiom</t>
+          <t>champinhom</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>plastrom</t>
+          <t>pistom</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>quirielêisom</t>
+          <t>acordeom</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>fonfom</t>
+          <t>infrassom</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>entretom</t>
+          <t>ano-bom</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>semitom</t>
+          <t>calom</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
+          <t>creiom</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>plastrom</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>quirielêisom</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>fonfom</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>entretom</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>semitom</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
           <t>raiom</t>
         </is>
       </c>
-      <c r="B16" t="inlineStr">
+      <c r="B17" t="inlineStr">
         <is>
           <t>ambom</t>
         </is>
       </c>
-      <c r="C16" t="inlineStr">
+      <c r="C17" t="inlineStr">
         <is>
           <t>dondom</t>
         </is>
       </c>
-      <c r="D16" t="inlineStr">
+      <c r="D17" t="inlineStr">
         <is>
           <t>candom</t>
         </is>
       </c>
-      <c r="E16" t="inlineStr">
+      <c r="E17" t="inlineStr">
         <is>
           <t>pororom</t>
         </is>
       </c>
-      <c r="F16" t="inlineStr">
+      <c r="F17" t="inlineStr">
         <is>
           <t>destom</t>
         </is>

</xml_diff>

<commit_message>
Ajustando e adicionando alguns tratamentos
</commit_message>
<xml_diff>
--- a/tabela_de_palavras.xlsx
+++ b/tabela_de_palavras.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F109"/>
+  <dimension ref="A1:E131"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -424,2631 +424,2221 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>chavão</t>
+          <t>destom</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>alienação</t>
+          <t>elucubração</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>desintegração</t>
+          <t>adesão</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>superação</t>
+          <t>proscrição</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>deflexão</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>intensão</t>
+          <t>punição</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>alegação</t>
+          <t>ereção</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>localização</t>
+          <t>putirom</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>dissensão</t>
+          <t>retificação</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>confirmação</t>
+          <t>especulação</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>decomposição</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>validação</t>
+          <t>grilhão</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>corrupção</t>
+          <t>apresentação</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>ribeirão</t>
+          <t>infração</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>aguilhão</t>
+          <t>malcriação</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>coação</t>
+          <t>bipolarização</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>reclamação</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>percussão</t>
+          <t>obstinação</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>palavrão</t>
+          <t>enumeração</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>anfitrião</t>
+          <t>denominação</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>distribuição</t>
+          <t>interação</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>indenização</t>
+          <t>dedicação</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>subscrição</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>aversão</t>
+          <t>expedição</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>trom</t>
+          <t>mutação</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>coesão</t>
+          <t>vulcão</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>refração</t>
+          <t>caperom</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>garçom</t>
+          <t>florão</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>colonização</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>extensão</t>
+          <t>rufião</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>erupção</t>
+          <t>caminhão</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>ressurreição</t>
+          <t>colaboração</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>fanfarrão</t>
+          <t>difusão</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>confissão</t>
+          <t>compreensão</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>insatisfação</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>ingestão</t>
+          <t>meisom</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>mobilização</t>
+          <t>tradução</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>plantão</t>
+          <t>inserção</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>postergação</t>
+          <t>sugestão</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>quirielêisom</t>
+          <t>distensão</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>nom</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>remissão</t>
+          <t>compressão</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>tradução</t>
+          <t>estatização</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>readequação</t>
+          <t>valorização</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>exerção</t>
+          <t>centurião</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>sensação</t>
+          <t>exortação</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>batom</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>descriminalização</t>
+          <t>imolação</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>pensão</t>
+          <t>distorção</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>abrasão</t>
+          <t>concisão</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>locomoção</t>
+          <t>competição</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>invasão</t>
+          <t>designação</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>consecução</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>pretensão</t>
+          <t>erudição</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>submersão</t>
+          <t>dilapidação</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>difusão</t>
+          <t>dabom</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>consolação</t>
+          <t>pensão</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>deprecação</t>
+          <t>ruamom</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>ambição</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>devoção</t>
+          <t>acusação</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>cupom</t>
+          <t>ressocialização</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>zonzom</t>
+          <t>acordeom</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>empolgação</t>
+          <t>heteroagressão</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>expansão</t>
+          <t>estagnação</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>abjeção</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>antemão</t>
+          <t>conexão</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>elevação</t>
+          <t>condição</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>supressão</t>
+          <t>ebulição</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>aspersão</t>
+          <t>desestatização</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>ruamom</t>
+          <t>cooptação</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>demarcação</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>bonotom</t>
+          <t>autorização</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>intelecção</t>
+          <t>conversão</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>utilização</t>
+          <t>adulação</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>pororom</t>
+          <t>inter-relação</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>infrassom</t>
+          <t>proposição</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>televisão</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>retratação</t>
+          <t>acomodação</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>destruição</t>
+          <t>prestidigitação</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>obstinação</t>
+          <t>dissensão</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>sanção</t>
+          <t>unção</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>capacitação</t>
+          <t>contensão</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>privatização</t>
-        </is>
-      </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>corporação</t>
+          <t>depredação</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>eleição</t>
+          <t>condensação</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>condom</t>
+          <t>afecção</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>concessão</t>
+          <t>lotação</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>sivom</t>
+          <t>conecção</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>burbom</t>
-        </is>
-      </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>comunicação</t>
+          <t>rejeição</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>quarteirão</t>
+          <t>precisão</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>deturpação</t>
+          <t>valoração</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>convicção</t>
+          <t>exclusão</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>unção</t>
+          <t>insurreição</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>reinauguração</t>
-        </is>
-      </c>
-      <c r="F16" t="inlineStr">
-        <is>
-          <t>bonachão</t>
+          <t>sedução</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>dom</t>
+          <t>aspersão</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>administração</t>
+          <t>quirielêisom</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>putirom</t>
+          <t>rerratificação</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>intonação</t>
+          <t>missão</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>aquisição</t>
-        </is>
-      </c>
-      <c r="F17" t="inlineStr">
-        <is>
-          <t>torrão</t>
+          <t>religião</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>leilão</t>
+          <t>infusão</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>contextualização</t>
+          <t>hissom</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>emissão</t>
+          <t>razão</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>extroversão</t>
+          <t>difamação</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>composição</t>
-        </is>
-      </c>
-      <c r="F18" t="inlineStr">
-        <is>
-          <t>imolação</t>
+          <t>emigração</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>instituição</t>
+          <t>suposição</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>supetão</t>
+          <t>mutom</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>caperom</t>
+          <t>delimitação</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>usurpação</t>
+          <t>encenação</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>conformação</t>
-        </is>
-      </c>
-      <c r="F19" t="inlineStr">
-        <is>
-          <t>intermediação</t>
+          <t>constituição</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>encenação</t>
+          <t>licitação</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>lacração</t>
+          <t>artesão</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>adesão</t>
+          <t>champinhom</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>enumeração</t>
+          <t>mobilização</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>malcriação</t>
-        </is>
-      </c>
-      <c r="F20" t="inlineStr">
-        <is>
-          <t>diatom</t>
+          <t>diversificação</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>estigmatização</t>
+          <t>sublimação</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>agregação</t>
+          <t>dom</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>conservação</t>
+          <t>citação</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>interlocução</t>
+          <t>decepção</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>ablação</t>
-        </is>
-      </c>
-      <c r="F21" t="inlineStr">
-        <is>
-          <t>interpolação</t>
+          <t>terceirização</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>veneração</t>
+          <t>exasperação</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>aprovação</t>
+          <t>gestação</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>indagação</t>
+          <t>marrom</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>vazão</t>
+          <t>reinauguração</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>solicitação</t>
-        </is>
-      </c>
-      <c r="F22" t="inlineStr">
-        <is>
-          <t>satisfação</t>
+          <t>brasão</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>conecção</t>
+          <t>vacilão</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>coleção</t>
+          <t>muxirom</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>concidadão</t>
+          <t>salvação</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>showroom</t>
+          <t>shalom</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>função</t>
-        </is>
-      </c>
-      <c r="F23" t="inlineStr">
-        <is>
-          <t>conexão</t>
+          <t>estimação</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>extradição</t>
+          <t>elaboração</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>delação</t>
+          <t>intenção</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>distorção</t>
+          <t>formulação</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>violação</t>
+          <t>bombom</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>guarnição</t>
-        </is>
-      </c>
-      <c r="F24" t="inlineStr">
-        <is>
-          <t>parlapatão</t>
+          <t>proclamação</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>bufão</t>
+          <t>isenção</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>inclinação</t>
+          <t>sultão</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>champinhom</t>
+          <t>bordão</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>intromissão</t>
+          <t>pregão</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>invenção</t>
-        </is>
-      </c>
-      <c r="F25" t="inlineStr">
-        <is>
-          <t>interação</t>
+          <t>regressão</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>precarização</t>
+          <t>opinião</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>consideração</t>
+          <t>raiom</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>lotação</t>
+          <t>sairão</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>presunção</t>
+          <t>reputação</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>subseção</t>
-        </is>
-      </c>
-      <c r="F26" t="inlineStr">
-        <is>
-          <t>afeição</t>
+          <t>estarão</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>sublimação</t>
+          <t>infrassom</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>explanação</t>
+          <t>gratidão</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>insurreição</t>
+          <t>retroalimentação</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>irrisão</t>
+          <t>inspiração</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>retidão</t>
-        </is>
-      </c>
-      <c r="F27" t="inlineStr">
-        <is>
-          <t>confederação</t>
+          <t>nom</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>seleção</t>
+          <t>contemplação</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>compaixão</t>
+          <t>massificação</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>absolvição</t>
+          <t>composição</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>raiom</t>
+          <t>insubordinação</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>zoom</t>
-        </is>
-      </c>
-      <c r="F28" t="inlineStr">
-        <is>
-          <t>retroalimentação</t>
+          <t>indagação</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>inter-relação</t>
+          <t>coabitação</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>cidadão</t>
+          <t>invenção</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>situação</t>
+          <t>retidão</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>vão</t>
+          <t>intermediação</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>iândom</t>
-        </is>
-      </c>
-      <c r="F29" t="inlineStr">
-        <is>
-          <t>higienização</t>
+          <t>showroom</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>regressão</t>
+          <t>depleção</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>prestação</t>
+          <t>intuição</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>missão</t>
+          <t>situação</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>execração</t>
+          <t>contração</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>bombom</t>
-        </is>
-      </c>
-      <c r="F30" t="inlineStr">
-        <is>
-          <t>captação</t>
+          <t>devoção</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>inspiração</t>
+          <t>concussão</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>relação</t>
+          <t>som</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>correção</t>
+          <t>ação</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>aspiração</t>
+          <t>aguilhão</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>interiorização</t>
-        </is>
-      </c>
-      <c r="F31" t="inlineStr">
-        <is>
-          <t>bordão</t>
+          <t>progressão</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>padrão</t>
+          <t>torrão</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>deposição</t>
+          <t>interiorização</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>escalão</t>
+          <t>seleção</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>aculturação</t>
+          <t>condução</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>ultrassom</t>
-        </is>
-      </c>
-      <c r="F32" t="inlineStr">
-        <is>
-          <t>autorização</t>
+          <t>espigão</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>prossecução</t>
+          <t>correção</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>interjeição</t>
+          <t>lesão</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>competição</t>
+          <t>palavrão</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>impressão</t>
+          <t>execução</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>tripulação</t>
-        </is>
-      </c>
-      <c r="F33" t="inlineStr">
-        <is>
-          <t>autoafirmação</t>
+          <t>estilização</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>pistom</t>
+          <t>extradição</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>tributação</t>
+          <t>compaixão</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>coração</t>
+          <t>certidão</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>discriminação</t>
+          <t>conservação</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>afecção</t>
-        </is>
-      </c>
-      <c r="F34" t="inlineStr">
-        <is>
-          <t>desoneração</t>
+          <t>restituição</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>especulação</t>
+          <t>postergação</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>sacralização</t>
+          <t>substituição</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>extirpação</t>
+          <t>transição</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>congratulação</t>
+          <t>arguição</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>lamentação</t>
-        </is>
-      </c>
-      <c r="F35" t="inlineStr">
-        <is>
-          <t>então</t>
+          <t>instalação</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>incorporação</t>
+          <t>justificação</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>tribulação</t>
+          <t>congratulação</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>omissão</t>
+          <t>empolgação</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>terceirização</t>
+          <t>segregação</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>violão</t>
-        </is>
-      </c>
-      <c r="F36" t="inlineStr">
-        <is>
-          <t>normatização</t>
+          <t>paixão</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>tom</t>
+          <t>alusão</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>acusação</t>
+          <t>masturbação</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>abolição</t>
+          <t>tributação</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>sofisticação</t>
+          <t>edição</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>mutirom</t>
-        </is>
-      </c>
-      <c r="F37" t="inlineStr">
-        <is>
-          <t>atração</t>
+          <t>complicação</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>verão</t>
+          <t>remissão</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>edição</t>
+          <t>expressão</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>corrimão</t>
+          <t>confissão</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>ligação</t>
+          <t>ingestão</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>facção</t>
-        </is>
-      </c>
-      <c r="F38" t="inlineStr">
-        <is>
-          <t>em vão</t>
+          <t>utilização</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>atribulação</t>
+          <t>convenção</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>plastrom</t>
+          <t>reverberação</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>bem-bom</t>
+          <t>erupção</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>discussão</t>
+          <t>restrição</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>desmobilização</t>
-        </is>
-      </c>
-      <c r="F39" t="inlineStr">
-        <is>
-          <t>serração</t>
+          <t>fragmentação</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>problematização</t>
+          <t>anfitrião</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>aflição</t>
+          <t>granulação</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>emigração</t>
+          <t>federação</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>projeção</t>
+          <t>usurpação</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>jetom</t>
-        </is>
-      </c>
-      <c r="F40" t="inlineStr">
-        <is>
-          <t>flexão</t>
+          <t>deliberação</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>marrom</t>
+          <t>comunicação</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>explosão</t>
+          <t>exemplificação</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>condensação</t>
+          <t>contraindicação</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>compreensão</t>
+          <t>lacração</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>dedicação</t>
-        </is>
-      </c>
-      <c r="F41" t="inlineStr">
-        <is>
-          <t>inclusão</t>
+          <t>demão</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>educação</t>
+          <t>estigmatização</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>percepção</t>
+          <t>plantão</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>tamom</t>
+          <t>relação</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>imbricação</t>
+          <t>dimensão</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>requisição</t>
-        </is>
-      </c>
-      <c r="F42" t="inlineStr">
-        <is>
-          <t>creiom</t>
+          <t>instituição</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>apreensão</t>
+          <t>sacralização</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>masturbação</t>
+          <t>afeição</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>planificação</t>
+          <t>idealização</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>são</t>
+          <t>confederação</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>cooptação</t>
-        </is>
-      </c>
-      <c r="F43" t="inlineStr">
-        <is>
-          <t>inauguração</t>
+          <t>interdição</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>expedição</t>
+          <t>cupom</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>semitom</t>
+          <t>explosão</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>atenção</t>
+          <t>inauguração</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>cessão</t>
+          <t>apropriação</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>dessacralização</t>
-        </is>
-      </c>
-      <c r="F44" t="inlineStr">
-        <is>
-          <t>murmuração</t>
+          <t>jetom</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>transformação</t>
+          <t>subscrição</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>escrivão</t>
+          <t>conspiração</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>edredom</t>
+          <t>conformação</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>restituição</t>
+          <t>verão</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>exteriorização</t>
-        </is>
-      </c>
-      <c r="F45" t="inlineStr">
-        <is>
-          <t>expressão</t>
+          <t>concessão</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>embrião</t>
+          <t>disposição</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>exibição</t>
+          <t>ascensão</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>justificação</t>
+          <t>armagedom</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>imersão</t>
+          <t>ressurreição</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>inserção</t>
-        </is>
-      </c>
-      <c r="F46" t="inlineStr">
-        <is>
-          <t>infração</t>
+          <t>intromissão</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>modificação</t>
+          <t>ambom</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>delimitação</t>
+          <t>alimentação</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>moletom</t>
+          <t>translação</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>compulsão</t>
+          <t>escrivão</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>acomodação</t>
-        </is>
-      </c>
-      <c r="F47" t="inlineStr">
-        <is>
-          <t>dongolodrom</t>
+          <t>escalão</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>intersecção</t>
+          <t>superação</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>execução</t>
+          <t>explanação</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>imprecação</t>
+          <t>cidadão</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>concatenação</t>
+          <t>compulsão</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>disseminação</t>
-        </is>
-      </c>
-      <c r="F48" t="inlineStr">
-        <is>
-          <t>companhom</t>
+          <t>batom</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>dominação</t>
+          <t>congregação</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>contraindicação</t>
+          <t>pompom</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>intercessão</t>
+          <t>obliteração</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>precisão</t>
+          <t>sofisticação</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>conceição</t>
-        </is>
-      </c>
-      <c r="F49" t="inlineStr">
-        <is>
-          <t>guidom</t>
+          <t>com</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>comunhão</t>
+          <t>malversação</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>estimação</t>
+          <t>constrição</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>recordação</t>
+          <t>ultrassom</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>deliberação</t>
+          <t>ministração</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>calom</t>
-        </is>
-      </c>
-      <c r="F50" t="inlineStr">
-        <is>
-          <t>muxirom</t>
+          <t>leilão</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>hissom</t>
+          <t>moletom</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>meisom</t>
+          <t>distribuição</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>confecção</t>
+          <t>emersão</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>congregação</t>
+          <t>vinculação</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>ilação</t>
-        </is>
-      </c>
-      <c r="F51" t="inlineStr">
-        <is>
-          <t>acordeom</t>
+          <t>persuasão</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>formulação</t>
+          <t>consolidação</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>conversação</t>
+          <t>abolição</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>afirmação</t>
+          <t>depreciação</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>transgressão</t>
+          <t>humanização</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>ambom</t>
-        </is>
-      </c>
-      <c r="F52" t="inlineStr">
-        <is>
-          <t>complicação</t>
+          <t>caramomom</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>pregão</t>
+          <t>então</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>puchom</t>
+          <t>conotação</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>excursão</t>
+          <t>execração</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>subversão</t>
+          <t>aprovação</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>panteão</t>
-        </is>
-      </c>
-      <c r="F53" t="inlineStr">
-        <is>
-          <t>emulação</t>
+          <t>extroversão</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>candom</t>
+          <t>assunção</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>certidão</t>
+          <t>ampliação</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>fomentação</t>
+          <t>cerração</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>sugestão</t>
+          <t>reprodução</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>intervenção</t>
-        </is>
-      </c>
-      <c r="F54" t="inlineStr">
-        <is>
-          <t>exceção</t>
+          <t>corrupção</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>remasterização</t>
+          <t>iândom</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>escolarização</t>
+          <t>aluvião</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>feição</t>
+          <t>atribulação</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>dissipação</t>
+          <t>ocupação</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>instauração</t>
-        </is>
-      </c>
-      <c r="F55" t="inlineStr">
-        <is>
-          <t>retaliação</t>
+          <t>apreensão</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>armagedom</t>
+          <t>ermitão</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>emoção</t>
+          <t>dongolodrom</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>distinção</t>
+          <t>deposição</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>diversificação</t>
+          <t>ligação</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>contradição</t>
-        </is>
-      </c>
-      <c r="F56" t="inlineStr">
-        <is>
-          <t>exclusão</t>
+          <t>concatenação</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>obsessão</t>
+          <t>são</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>ronrom</t>
+          <t>pororom</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>coisificação</t>
+          <t>inadequação</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>contração</t>
+          <t>campeão</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>publicização</t>
-        </is>
-      </c>
-      <c r="F57" t="inlineStr">
-        <is>
-          <t>obliteração</t>
+          <t>rotação</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>proposição</t>
+          <t>privatização</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>secessão</t>
+          <t>delegação</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>quitação</t>
+          <t>ano-bom</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>locação</t>
+          <t>distinção</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>fonfom</t>
-        </is>
-      </c>
-      <c r="F58" t="inlineStr">
-        <is>
-          <t>banalização</t>
+          <t>educação</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>progressão</t>
+          <t>contramão</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>determinação</t>
+          <t>privação</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>subdivisão</t>
+          <t>quinhão</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>discrição</t>
+          <t>abstração</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>aglutinação</t>
-        </is>
-      </c>
-      <c r="F59" t="inlineStr">
-        <is>
-          <t>pompom</t>
+          <t>colação</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>ampliação</t>
+          <t>exerção</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>depuração</t>
+          <t>ingratidão</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>exemplificação</t>
+          <t>ancião</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>aluvião</t>
+          <t>intercessão</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>mutom</t>
-        </is>
-      </c>
-      <c r="F60" t="inlineStr">
-        <is>
-          <t>definição</t>
+          <t>guarnição</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>rotação</t>
+          <t>comunhão</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>autoavaliação</t>
+          <t>elação</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>abnegação</t>
+          <t>puchom</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>exasperação</t>
+          <t>requisição</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>defecção</t>
-        </is>
-      </c>
-      <c r="F61" t="inlineStr">
-        <is>
-          <t>divulgação</t>
+          <t>bom</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>vulcão</t>
+          <t>deprecação</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>pavimentação</t>
+          <t>regeneração</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>razão</t>
+          <t>secção</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>denominação</t>
+          <t>obsessão</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>contensão</t>
-        </is>
-      </c>
-      <c r="F62" t="inlineStr">
-        <is>
-          <t>condução</t>
+          <t>contradição</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>sótão</t>
+          <t>santom</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>caramomom</t>
+          <t>informação</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>mutirão</t>
+          <t>resolução</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>abstração</t>
+          <t>abnegação</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>lesão</t>
-        </is>
-      </c>
-      <c r="F63" t="inlineStr">
-        <is>
-          <t>constituição</t>
+          <t>aspiração</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>religião</t>
+          <t>protrusão</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>habitação</t>
+          <t>abrasão</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>bom</t>
+          <t>celebração</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>escuridão</t>
+          <t>predestinação</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>obipom</t>
-        </is>
-      </c>
-      <c r="F64" t="inlineStr">
-        <is>
-          <t>estação</t>
+          <t>botão</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>rufião</t>
+          <t>oposição</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>pogrom</t>
+          <t>mutirão</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>dabom</t>
+          <t>abjeção</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>subjugação</t>
+          <t>feição</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>barão</t>
-        </is>
-      </c>
-      <c r="F65" t="inlineStr">
-        <is>
-          <t>ministração</t>
+          <t>parlapatão</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>decepção</t>
+          <t>modificação</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>detração</t>
+          <t>pavimentação</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>valorização</t>
+          <t>cessão</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>grão</t>
+          <t>sanção</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>conversão</t>
-        </is>
-      </c>
-      <c r="F66" t="inlineStr">
-        <is>
-          <t>introdução</t>
+          <t>mitigação</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>artesão</t>
+          <t>zoom</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>salvação</t>
+          <t>fruição</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>limão</t>
+          <t>imissão</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>instalação</t>
+          <t>repetição</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>dondom</t>
-        </is>
-      </c>
-      <c r="F67" t="inlineStr">
-        <is>
-          <t>reputação</t>
+          <t>submersão</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>intenção</t>
+          <t>introdução</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>ressocialização</t>
+          <t>habitação</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>alusão</t>
+          <t>eleição</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>questão</t>
+          <t>subversão</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>fornicação</t>
-        </is>
-      </c>
-      <c r="F68" t="inlineStr">
-        <is>
-          <t>meditação</t>
+          <t>incorporação</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>adjudicação</t>
+          <t>dicção</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>órgão</t>
+          <t>murmuração</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>imaginação</t>
+          <t>violação</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>restrição</t>
+          <t>deturpação</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>demão</t>
-        </is>
-      </c>
-      <c r="F69" t="inlineStr">
-        <is>
-          <t>resolução</t>
+          <t>barão</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>rejeição</t>
+          <t>condom</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>som</t>
+          <t>semitom</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>agressão</t>
+          <t>ordenação</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>estilização</t>
+          <t>vazão</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>canastrão</t>
-        </is>
-      </c>
-      <c r="F70" t="inlineStr">
-        <is>
-          <t>constipação</t>
+          <t>convicção</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>grilhão</t>
+          <t>quitação</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>repleção</t>
+          <t>absolvição</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>charlatão</t>
+          <t>expansão</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>contemplação</t>
+          <t>violão</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>concepção</t>
-        </is>
-      </c>
-      <c r="F71" t="inlineStr">
-        <is>
-          <t>asserção</t>
+          <t>desoneração</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>aproximação</t>
+          <t>sessão</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>paixão</t>
+          <t>fonfom</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>conotação</t>
+          <t>imprecisão</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>interdição</t>
+          <t>alçapão</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>vacilão</t>
-        </is>
-      </c>
-      <c r="F72" t="inlineStr">
-        <is>
-          <t>potirom</t>
+          <t>fanfarrão</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>difamação</t>
+          <t>tenção</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>submissão</t>
+          <t>seção</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>regeneração</t>
+          <t>invasão</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>campeão</t>
+          <t>delação</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>botão</t>
-        </is>
-      </c>
-      <c r="F73" t="inlineStr">
-        <is>
-          <t>apresentação</t>
+          <t>limão</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>acepção</t>
+          <t>satisfação</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>simulação</t>
+          <t>estandardização</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>verificação</t>
+          <t>padrão</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>prestidigitação</t>
+          <t>detenção</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>incubação</t>
-        </is>
-      </c>
-      <c r="F74" t="inlineStr">
-        <is>
-          <t>macarrão</t>
+          <t>inclinação</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>denotação</t>
+          <t>colonização</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>menção</t>
+          <t>coleção</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>protrusão</t>
+          <t>desintegração</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>retroação</t>
+          <t>prossecução</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>aptidão</t>
-        </is>
-      </c>
-      <c r="F75" t="inlineStr">
-        <is>
-          <t>atribuição</t>
+          <t>integração</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>gibão</t>
+          <t>defecção</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>shalom</t>
+          <t>recreação</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>laceração</t>
+          <t>função</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>premonição</t>
+          <t>aptidão</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>opinião</t>
-        </is>
-      </c>
-      <c r="F76" t="inlineStr">
-        <is>
-          <t>reivindicação</t>
+          <t>transformação</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>imprecisão</t>
+          <t>validação</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>união</t>
+          <t>canção</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>desagregação</t>
+          <t>autoafirmação</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>massificação</t>
+          <t>balão</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>persuasão</t>
-        </is>
-      </c>
-      <c r="F77" t="inlineStr">
-        <is>
-          <t>abdicação</t>
+          <t>antecipação</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>conciliação</t>
+          <t>pogrom</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>fragmentação</t>
+          <t>fração</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>glonglom</t>
+          <t>problematização</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>mitigação</t>
+          <t>califom</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>infusão</t>
-        </is>
-      </c>
-      <c r="F78" t="inlineStr">
-        <is>
-          <t>importunação</t>
+          <t>precarização</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>com</t>
+          <t>secessão</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>fascinação</t>
+          <t>entretom</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>contenção</t>
+          <t>corrimão</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>concussão</t>
+          <t>potirom</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>celebração</t>
-        </is>
-      </c>
-      <c r="F79" t="inlineStr">
-        <is>
-          <t>consolidação</t>
+          <t>imprecação</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>comutação</t>
+          <t>dissipação</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>quinhão</t>
+          <t>alienação</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>degradação</t>
+          <t>aversão</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>separação</t>
+          <t>estação</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>califom</t>
-        </is>
-      </c>
-      <c r="F80" t="inlineStr">
-        <is>
-          <t>delegação</t>
+          <t>interrupção</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>ano-bom</t>
+          <t>conceição</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>sultão</t>
+          <t>retroação</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>licitação</t>
+          <t>enunciação</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>extração</t>
+          <t>burbom</t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>translação</t>
-        </is>
-      </c>
-      <c r="F81" t="inlineStr">
-        <is>
-          <t>conflagração</t>
+          <t>extorsão</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>elisão</t>
+          <t>intonação</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>insubordinação</t>
+          <t>craiom</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>dilapidação</t>
+          <t>institucionalização</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>colação</t>
+          <t>resignação</t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>gestação</t>
-        </is>
-      </c>
-      <c r="F82" t="inlineStr">
-        <is>
-          <t>resignação</t>
+          <t>pericom</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>reflexão</t>
+          <t>asserção</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
@@ -3058,148 +2648,123 @@
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>capitão</t>
+          <t>pretensão</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>demonstração</t>
+          <t>conflagração</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>proclamação</t>
-        </is>
-      </c>
-      <c r="F83" t="inlineStr">
-        <is>
-          <t>organização</t>
+          <t>aculturação</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>depreciação</t>
+          <t>tripulação</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>ascensão</t>
+          <t>imaginação</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>prostituição</t>
+          <t>afirmação</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>tição</t>
+          <t>subjugação</t>
         </is>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>ação</t>
-        </is>
-      </c>
-      <c r="F84" t="inlineStr">
-        <is>
-          <t>redenção</t>
+          <t>vão</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>craiom</t>
+          <t>grão</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>elucubração</t>
+          <t>percepção</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>reverberação</t>
+          <t>incubação</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>idealização</t>
+          <t>interlocução</t>
         </is>
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>retificação</t>
-        </is>
-      </c>
-      <c r="F85" t="inlineStr">
-        <is>
-          <t>constrição</t>
+          <t>separação</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>adulação</t>
+          <t>planificação</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>condição</t>
+          <t>locomoção</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>pericom</t>
+          <t>lamentação</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>humanização</t>
+          <t>fascinação</t>
         </is>
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>coerção</t>
-        </is>
-      </c>
-      <c r="F86" t="inlineStr">
-        <is>
-          <t>disposição</t>
+          <t>indiscrição</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>crepom</t>
+          <t>coação</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>citação</t>
+          <t>canalização</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>antecipação</t>
+          <t>recordação</t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>punição</t>
+          <t>recomendação</t>
         </is>
       </c>
       <c r="E87" t="inlineStr">
-        <is>
-          <t>pressão</t>
-        </is>
-      </c>
-      <c r="F87" t="inlineStr">
         <is>
           <t>contrafação</t>
         </is>
@@ -3208,704 +2773,1188 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>qualificação</t>
+          <t>inclusão</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>excepção</t>
+          <t>prolação</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>depleção</t>
+          <t>dissolução</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>concisão</t>
+          <t>descrição</t>
         </is>
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>fração</t>
-        </is>
-      </c>
-      <c r="F88" t="inlineStr">
-        <is>
-          <t>ereção</t>
+          <t>anzom</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>visão</t>
+          <t>concepção</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>segregação</t>
+          <t>atenuação</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>revisão</t>
+          <t>fomentação</t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>coabitação</t>
+          <t>consecução</t>
         </is>
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>isenção</t>
-        </is>
-      </c>
-      <c r="F89" t="inlineStr">
-        <is>
-          <t>sedução</t>
+          <t>impressão</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>dissolução</t>
+          <t>regulamentação</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>reprodução</t>
+          <t>capitão</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>recuperação</t>
+          <t>decisão</t>
         </is>
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>malversação</t>
+          <t>laceração</t>
         </is>
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>bipolarização</t>
-        </is>
-      </c>
-      <c r="F90" t="inlineStr">
-        <is>
-          <t>contramão</t>
+          <t>escuridão</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>ebulição</t>
+          <t>subseção</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>dicção</t>
+          <t>capacitação</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>autorregulação</t>
+          <t>contraprestação</t>
         </is>
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>erudição</t>
+          <t>televisão</t>
         </is>
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>detenção</t>
-        </is>
-      </c>
-      <c r="F91" t="inlineStr">
-        <is>
-          <t>combinação</t>
+          <t>quarteirão</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>inadequação</t>
+          <t>mutirom</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>tenção</t>
+          <t>normatização</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>equiparação</t>
+          <t>coerção</t>
         </is>
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>racionalização</t>
+          <t>extração</t>
         </is>
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>provisão</t>
-        </is>
-      </c>
-      <c r="F92" t="inlineStr">
-        <is>
-          <t>estandardização</t>
+          <t>confirmação</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>prospecção</t>
+          <t>autoavaliação</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>contraprestação</t>
+          <t>sensação</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>preterição</t>
+          <t>ambição</t>
         </is>
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>suposição</t>
+          <t>trom</t>
         </is>
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>retenção</t>
-        </is>
-      </c>
-      <c r="F93" t="inlineStr">
-        <is>
-          <t>alimentação</t>
+          <t>charlatão</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>predestinação</t>
+          <t>tamom</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>distensão</t>
+          <t>concidadão</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>exposição</t>
+          <t>coisificação</t>
         </is>
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>ordenação</t>
+          <t>constipação</t>
         </is>
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>repetição</t>
-        </is>
-      </c>
-      <c r="F94" t="inlineStr">
-        <is>
-          <t>estagnação</t>
+          <t>visão</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>interrupção</t>
+          <t>instauração</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>caminhão</t>
+          <t>projeção</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>cagom</t>
+          <t>fornicação</t>
         </is>
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>anzom</t>
+          <t>macarrão</t>
         </is>
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>emersão</t>
-        </is>
-      </c>
-      <c r="F95" t="inlineStr">
-        <is>
-          <t>cerração</t>
+          <t>filão</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>descrição</t>
+          <t>reclamação</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>boom</t>
+          <t>aglutinação</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>rerratificação</t>
+          <t>ilação</t>
         </is>
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>imissão</t>
+          <t>atenção</t>
         </is>
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>santom</t>
-        </is>
-      </c>
-      <c r="F96" t="inlineStr">
-        <is>
-          <t>brasão</t>
+          <t>qualificação</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>balão</t>
+          <t>solicitação</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>admoestação</t>
+          <t>emoção</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>heteroagressão</t>
+          <t>embrião</t>
         </is>
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>compressão</t>
+          <t>facção</t>
         </is>
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>comissão</t>
-        </is>
-      </c>
-      <c r="F97" t="inlineStr">
-        <is>
-          <t>mutação</t>
+          <t>ruralização</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>homem-bom</t>
+          <t>equiparação</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>depredação</t>
+          <t>recuperação</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>ancião</t>
+          <t>retratação</t>
         </is>
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>canção</t>
+          <t>reivindicação</t>
         </is>
       </c>
       <c r="E98" t="inlineStr">
         <is>
-          <t>recomendação</t>
-        </is>
-      </c>
-      <c r="F98" t="inlineStr">
-        <is>
-          <t>convenção</t>
+          <t>pistom</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>indiscrição</t>
+          <t>maçom</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>fruição</t>
+          <t>imersão</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>designação</t>
+          <t>aflição</t>
         </is>
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>ruralização</t>
+          <t>indenização</t>
         </is>
       </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t>privação</t>
-        </is>
-      </c>
-      <c r="F99" t="inlineStr">
-        <is>
-          <t>decisão</t>
+          <t>inovação</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>preparaçã</t>
+          <t>intervenção</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>estarão</t>
+          <t>crepom</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>mistificação</t>
+          <t>agregação</t>
         </is>
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>ponderação</t>
+          <t>cão</t>
         </is>
       </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t>proscrição</t>
-        </is>
-      </c>
-      <c r="F100" t="inlineStr">
-        <is>
-          <t>inovação</t>
+          <t>conversação</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>valoração</t>
+          <t>intersecção</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>condecoração</t>
+          <t>elocução</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>perturbação</t>
+          <t>antemão</t>
         </is>
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>glom</t>
+          <t>glonglom</t>
         </is>
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t>regulamentação</t>
-        </is>
-      </c>
-      <c r="F101" t="inlineStr">
-        <is>
-          <t>vedação</t>
+          <t>preterição</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>contextualização</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>integração</t>
+          <t>emissão</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>institucionalização</t>
+          <t>admoestação</t>
         </is>
       </c>
       <c r="D102" t="inlineStr">
         <is>
-          <t>conspiração</t>
+          <t>submissão</t>
         </is>
       </c>
       <c r="E102" t="inlineStr">
         <is>
-          <t>desestatização</t>
-        </is>
-      </c>
-      <c r="F102" t="inlineStr">
-        <is>
-          <t>elaboração</t>
+          <t>publicização</t>
         </is>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>entretom</t>
+          <t>tição</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>dimensão</t>
+          <t>sivom</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>sairão</t>
+          <t>elisão</t>
         </is>
       </c>
       <c r="D103" t="inlineStr">
         <is>
-          <t>oposição</t>
+          <t>discrição</t>
         </is>
       </c>
       <c r="E103" t="inlineStr">
         <is>
-          <t>canalização</t>
-        </is>
-      </c>
-      <c r="F103" t="inlineStr">
-        <is>
-          <t>interrogação</t>
+          <t>programação</t>
         </is>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>elocução</t>
+          <t>interrogação</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>intuição</t>
+          <t>detração</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>seção</t>
+          <t>comutação</t>
         </is>
       </c>
       <c r="D104" t="inlineStr">
         <is>
-          <t>apreciação</t>
+          <t>discussão</t>
         </is>
       </c>
       <c r="E104" t="inlineStr">
         <is>
-          <t>federação</t>
-        </is>
-      </c>
-      <c r="F104" t="inlineStr">
-        <is>
-          <t>maçom</t>
+          <t>obipom</t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>vinculação</t>
+          <t>imbricação</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>arguição</t>
+          <t>cagom</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>florão</t>
+          <t>chavão</t>
         </is>
       </c>
       <c r="D105" t="inlineStr">
         <is>
-          <t>apropriação</t>
+          <t>redenção</t>
         </is>
       </c>
       <c r="E105" t="inlineStr">
         <is>
-          <t>ocupação</t>
-        </is>
-      </c>
-      <c r="F105" t="inlineStr">
-        <is>
-          <t>filão</t>
+          <t>companhom</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>ermitão</t>
+          <t>divulgação</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>tecido de granulação</t>
+          <t>questão</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>estatização</t>
+          <t>vedação</t>
         </is>
       </c>
       <c r="D106" t="inlineStr">
         <is>
-          <t>elação</t>
+          <t>flexão</t>
         </is>
       </c>
       <c r="E106" t="inlineStr">
         <is>
-          <t>ingratidão</t>
-        </is>
-      </c>
-      <c r="F106" t="inlineStr">
-        <is>
-          <t>força de expressão</t>
+          <t>veneração</t>
         </is>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>gratidão</t>
+          <t>contenção</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>centurião</t>
+          <t>determinação</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>inscrição</t>
+          <t>aproximação</t>
         </is>
       </c>
       <c r="D107" t="inlineStr">
         <is>
-          <t>alçapão</t>
+          <t>decomposição</t>
         </is>
       </c>
       <c r="E107" t="inlineStr">
         <is>
-          <t>monção</t>
-        </is>
-      </c>
-      <c r="F107" t="inlineStr">
-        <is>
-          <t>secção</t>
+          <t>intensão</t>
         </is>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>exortação</t>
+          <t>confecção</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>espigão</t>
+          <t>readequação</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>transição</t>
+          <t>dominação</t>
         </is>
       </c>
       <c r="D108" t="inlineStr">
         <is>
-          <t>substituição</t>
+          <t>percussão</t>
         </is>
       </c>
       <c r="E108" t="inlineStr">
         <is>
-          <t>objeção</t>
-        </is>
-      </c>
-      <c r="F108" t="inlineStr">
-        <is>
-          <t>sessão</t>
+          <t>provisão</t>
         </is>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>extorsão</t>
+          <t>demonstração</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>assunção</t>
+          <t>retaliação</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>colaboração</t>
+          <t>destruição</t>
         </is>
       </c>
       <c r="D109" t="inlineStr">
         <is>
-          <t>atenuação</t>
+          <t>deflexão</t>
         </is>
       </c>
       <c r="E109" t="inlineStr">
         <is>
-          <t>enunciação</t>
-        </is>
-      </c>
-      <c r="F109" t="inlineStr">
-        <is>
-          <t>programação</t>
+          <t>excursão</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>edredom</t>
+        </is>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>ronrom</t>
+        </is>
+      </c>
+      <c r="C110" t="inlineStr">
+        <is>
+          <t>conciliação</t>
+        </is>
+      </c>
+      <c r="D110" t="inlineStr">
+        <is>
+          <t>gibão</t>
+        </is>
+      </c>
+      <c r="E110" t="inlineStr">
+        <is>
+          <t>mistificação</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>remasterização</t>
+        </is>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>consolação</t>
+        </is>
+      </c>
+      <c r="C111" t="inlineStr">
+        <is>
+          <t>serração</t>
+        </is>
+      </c>
+      <c r="D111" t="inlineStr">
+        <is>
+          <t>plastrom</t>
+        </is>
+      </c>
+      <c r="E111" t="inlineStr">
+        <is>
+          <t>bufão</t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>monção</t>
+        </is>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>locação</t>
+        </is>
+      </c>
+      <c r="C112" t="inlineStr">
+        <is>
+          <t>exteriorização</t>
+        </is>
+      </c>
+      <c r="D112" t="inlineStr">
+        <is>
+          <t>coesão</t>
+        </is>
+      </c>
+      <c r="E112" t="inlineStr">
+        <is>
+          <t>depuração</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>excepção</t>
+        </is>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>não</t>
+        </is>
+      </c>
+      <c r="C113" t="inlineStr">
+        <is>
+          <t>repleção</t>
+        </is>
+      </c>
+      <c r="D113" t="inlineStr">
+        <is>
+          <t>bonachão</t>
+        </is>
+      </c>
+      <c r="E113" t="inlineStr">
+        <is>
+          <t>apreciação</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>atribuição</t>
+        </is>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>bonotom</t>
+        </is>
+      </c>
+      <c r="C114" t="inlineStr">
+        <is>
+          <t>coração</t>
+        </is>
+      </c>
+      <c r="D114" t="inlineStr">
+        <is>
+          <t>alegação</t>
+        </is>
+      </c>
+      <c r="E114" t="inlineStr">
+        <is>
+          <t>tribulação</t>
+        </is>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>organização</t>
+        </is>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>captação</t>
+        </is>
+      </c>
+      <c r="C115" t="inlineStr">
+        <is>
+          <t>homem-bom</t>
+        </is>
+      </c>
+      <c r="D115" t="inlineStr">
+        <is>
+          <t>prestação</t>
+        </is>
+      </c>
+      <c r="E115" t="inlineStr">
+        <is>
+          <t>subdivisão</t>
+        </is>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>extirpação</t>
+        </is>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>creiom</t>
+        </is>
+      </c>
+      <c r="C116" t="inlineStr">
+        <is>
+          <t>corporação</t>
+        </is>
+      </c>
+      <c r="D116" t="inlineStr">
+        <is>
+          <t>banalização</t>
+        </is>
+      </c>
+      <c r="E116" t="inlineStr">
+        <is>
+          <t>bem-bom</t>
+        </is>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>canastrão</t>
+        </is>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>exceção</t>
+        </is>
+      </c>
+      <c r="C117" t="inlineStr">
+        <is>
+          <t>comissão</t>
+        </is>
+      </c>
+      <c r="D117" t="inlineStr">
+        <is>
+          <t>tom</t>
+        </is>
+      </c>
+      <c r="E117" t="inlineStr">
+        <is>
+          <t>discriminação</t>
+        </is>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>zonzom</t>
+        </is>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>menção</t>
+        </is>
+      </c>
+      <c r="C118" t="inlineStr">
+        <is>
+          <t>administração</t>
+        </is>
+      </c>
+      <c r="D118" t="inlineStr">
+        <is>
+          <t>importunação</t>
+        </is>
+      </c>
+      <c r="E118" t="inlineStr">
+        <is>
+          <t>calom</t>
+        </is>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>acepção</t>
+        </is>
+      </c>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t>supetão</t>
+        </is>
+      </c>
+      <c r="C119" t="inlineStr">
+        <is>
+          <t>disseminação</t>
+        </is>
+      </c>
+      <c r="D119" t="inlineStr">
+        <is>
+          <t>ribeirão</t>
+        </is>
+      </c>
+      <c r="E119" t="inlineStr">
+        <is>
+          <t>desmobilização</t>
+        </is>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>objeção</t>
+        </is>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>verificação</t>
+        </is>
+      </c>
+      <c r="C120" t="inlineStr">
+        <is>
+          <t>prospecção</t>
+        </is>
+      </c>
+      <c r="D120" t="inlineStr">
+        <is>
+          <t>meditação</t>
+        </is>
+      </c>
+      <c r="E120" t="inlineStr">
+        <is>
+          <t>descriminalização</t>
+        </is>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>combinação</t>
+        </is>
+      </c>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t>sótão</t>
+        </is>
+      </c>
+      <c r="C121" t="inlineStr">
+        <is>
+          <t>guidom</t>
+        </is>
+      </c>
+      <c r="D121" t="inlineStr">
+        <is>
+          <t>extensão</t>
+        </is>
+      </c>
+      <c r="E121" t="inlineStr">
+        <is>
+          <t>dondom</t>
+        </is>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="inlineStr">
+        <is>
+          <t>consideração</t>
+        </is>
+      </c>
+      <c r="B122" t="inlineStr">
+        <is>
+          <t>elevação</t>
+        </is>
+      </c>
+      <c r="C122" t="inlineStr">
+        <is>
+          <t>perturbação</t>
+        </is>
+      </c>
+      <c r="D122" t="inlineStr">
+        <is>
+          <t>presunção</t>
+        </is>
+      </c>
+      <c r="E122" t="inlineStr">
+        <is>
+          <t>pressão</t>
+        </is>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="inlineStr">
+        <is>
+          <t>demarcação</t>
+        </is>
+      </c>
+      <c r="B123" t="inlineStr">
+        <is>
+          <t>reflexão</t>
+        </is>
+      </c>
+      <c r="C123" t="inlineStr">
+        <is>
+          <t>omissão</t>
+        </is>
+      </c>
+      <c r="D123" t="inlineStr">
+        <is>
+          <t>irrisão</t>
+        </is>
+      </c>
+      <c r="E123" t="inlineStr">
+        <is>
+          <t>intelecção</t>
+        </is>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="inlineStr">
+        <is>
+          <t>ponderação</t>
+        </is>
+      </c>
+      <c r="B124" t="inlineStr">
+        <is>
+          <t>abdicação</t>
+        </is>
+      </c>
+      <c r="C124" t="inlineStr">
+        <is>
+          <t>união</t>
+        </is>
+      </c>
+      <c r="D124" t="inlineStr">
+        <is>
+          <t>condecoração</t>
+        </is>
+      </c>
+      <c r="E124" t="inlineStr">
+        <is>
+          <t>revisão</t>
+        </is>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="inlineStr">
+        <is>
+          <t>panteão</t>
+        </is>
+      </c>
+      <c r="B125" t="inlineStr">
+        <is>
+          <t>candom</t>
+        </is>
+      </c>
+      <c r="C125" t="inlineStr">
+        <is>
+          <t>adjudicação</t>
+        </is>
+      </c>
+      <c r="D125" t="inlineStr">
+        <is>
+          <t>atração</t>
+        </is>
+      </c>
+      <c r="E125" t="inlineStr">
+        <is>
+          <t>ablação</t>
+        </is>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="inlineStr">
+        <is>
+          <t>insatisfação</t>
+        </is>
+      </c>
+      <c r="B126" t="inlineStr">
+        <is>
+          <t>boom</t>
+        </is>
+      </c>
+      <c r="C126" t="inlineStr">
+        <is>
+          <t>higienização</t>
+        </is>
+      </c>
+      <c r="D126" t="inlineStr">
+        <is>
+          <t>autorregulação</t>
+        </is>
+      </c>
+      <c r="E126" t="inlineStr">
+        <is>
+          <t>garçom</t>
+        </is>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="inlineStr">
+        <is>
+          <t>retenção</t>
+        </is>
+      </c>
+      <c r="B127" t="inlineStr">
+        <is>
+          <t>racionalização</t>
+        </is>
+      </c>
+      <c r="C127" t="inlineStr">
+        <is>
+          <t>interjeição</t>
+        </is>
+      </c>
+      <c r="D127" t="inlineStr">
+        <is>
+          <t>inscrição</t>
+        </is>
+      </c>
+      <c r="E127" t="inlineStr">
+        <is>
+          <t>exibição</t>
+        </is>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="inlineStr">
+        <is>
+          <t>prostituição</t>
+        </is>
+      </c>
+      <c r="B128" t="inlineStr">
+        <is>
+          <t>interpolação</t>
+        </is>
+      </c>
+      <c r="C128" t="inlineStr">
+        <is>
+          <t>refração</t>
+        </is>
+      </c>
+      <c r="D128" t="inlineStr">
+        <is>
+          <t>definição</t>
+        </is>
+      </c>
+      <c r="E128" t="inlineStr">
+        <is>
+          <t>exposição</t>
+        </is>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="inlineStr">
+        <is>
+          <t>premonição</t>
+        </is>
+      </c>
+      <c r="B129" t="inlineStr">
+        <is>
+          <t>transgressão</t>
+        </is>
+      </c>
+      <c r="C129" t="inlineStr">
+        <is>
+          <t>degradação</t>
+        </is>
+      </c>
+      <c r="D129" t="inlineStr">
+        <is>
+          <t>simulação</t>
+        </is>
+      </c>
+      <c r="E129" t="inlineStr">
+        <is>
+          <t>escolarização</t>
+        </is>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="inlineStr">
+        <is>
+          <t>diatom</t>
+        </is>
+      </c>
+      <c r="B130" t="inlineStr">
+        <is>
+          <t>emulação</t>
+        </is>
+      </c>
+      <c r="C130" t="inlineStr">
+        <is>
+          <t>órgão</t>
+        </is>
+      </c>
+      <c r="D130" t="inlineStr">
+        <is>
+          <t>agressão</t>
+        </is>
+      </c>
+      <c r="E130" t="inlineStr">
+        <is>
+          <t>aquisição</t>
+        </is>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="inlineStr">
+        <is>
+          <t>glom</t>
+        </is>
+      </c>
+      <c r="B131" t="inlineStr">
+        <is>
+          <t>localização</t>
+        </is>
+      </c>
+      <c r="C131" t="inlineStr">
+        <is>
+          <t>desagregação</t>
+        </is>
+      </c>
+      <c r="D131" t="inlineStr">
+        <is>
+          <t>dessacralização</t>
+        </is>
+      </c>
+      <c r="E131" t="inlineStr">
+        <is>
+          <t>supressão</t>
         </is>
       </c>
     </row>

</xml_diff>